<commit_message>
time warp for example model from 2014 to 2021
</commit_message>
<xml_diff>
--- a/doc/examples/resource/resource-type.xlsx
+++ b/doc/examples/resource/resource-type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\community\doc\user-guide\cookbook\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\examples\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA999F50-20A4-47C1-B805-D197C41A8FAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="3398" windowWidth="17280" windowHeight="8963" tabRatio="946" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="buffer" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <sheet name="resource" sheetId="13" r:id="rId11"/>
     <sheet name="parameter" sheetId="19" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -268,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,23 +394,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -447,23 +429,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -639,16 +604,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -662,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -676,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -690,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -710,21 +675,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -765,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -786,7 +751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -809,7 +774,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -835,21 +800,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -880,7 +845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -894,7 +859,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -908,7 +873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -922,7 +887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -939,21 +904,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -964,18 +929,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="1">
-        <v>41640</v>
+        <v>44197</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -986,7 +951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1003,20 +968,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1025,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1104,12 +1069,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="1">
-        <v>41730</v>
+        <v>44287</v>
       </c>
       <c r="C3" s="1">
         <v>47848</v>
@@ -1148,15 +1113,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="1">
-        <v>41640</v>
+        <v>44197</v>
       </c>
       <c r="C4" s="1">
-        <v>42735</v>
+        <v>45291</v>
       </c>
       <c r="D4">
         <v>10000</v>
@@ -1198,19 +1163,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1226,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1234,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1248,24 +1213,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1276,21 +1241,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1322,7 +1287,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1336,7 +1301,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1">
-        <v>41640</v>
+        <v>44197</v>
       </c>
       <c r="F2" t="s">
         <v>30</v>
@@ -1354,7 +1319,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1368,7 +1333,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="1">
-        <v>41760</v>
+        <v>44317</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
@@ -1386,7 +1351,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1400,7 +1365,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="1">
-        <v>41852</v>
+        <v>44409</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
@@ -1424,22 +1389,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1453,7 +1418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1467,7 +1432,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1481,7 +1446,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1495,7 +1460,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1509,7 +1474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1523,7 +1488,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1543,35 +1508,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1582,21 +1547,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1607,7 +1572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1618,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1640,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1651,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1668,20 +1633,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>54</v>
       </c>

</xml_diff>